<commit_message>
Lab11 on SSE finished
</commit_message>
<xml_diff>
--- a/Physics_Labs/6_sem/Lab6112/data.xlsx
+++ b/Physics_Labs/6_sem/Lab6112/data.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24972C64-F45A-456A-ADF6-9F3EFADD31E0}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95444A15-7643-4DDD-A8F3-1AAA06FD6C93}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-8272" yWindow="6233" windowWidth="17512" windowHeight="13597" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="24496" windowHeight="15796" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -3898,8 +3898,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="F35" sqref="F35"/>
+    <sheetView tabSelected="1" topLeftCell="A39" zoomScale="117" workbookViewId="0">
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>

<commit_message>
Lab 4 on Computational Math finished
</commit_message>
<xml_diff>
--- a/Physics_Labs/6_sem/Lab6112/data.xlsx
+++ b/Physics_Labs/6_sem/Lab6112/data.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95444A15-7643-4DDD-A8F3-1AAA06FD6C93}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="30" documentId="13_ncr:1_{95444A15-7643-4DDD-A8F3-1AAA06FD6C93}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{88E7670A-923B-4E65-9ED5-61BC51CA279F}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="24496" windowHeight="15796" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="6795" yWindow="232" windowWidth="17513" windowHeight="13598" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -702,6 +702,56 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="exp"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.15951329597697134"/>
+                  <c:y val="5.8681960596888107E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="ru-RU"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
           <c:xVal>
             <c:numRef>
               <c:f>Лист1!$B$14:$B$56</c:f>
@@ -3898,8 +3948,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" zoomScale="117" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="117" workbookViewId="0">
+      <selection activeCell="E66" sqref="E66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -4163,7 +4213,7 @@
         <v>2500</v>
       </c>
       <c r="E16">
-        <f t="shared" ref="E16:E41" si="1">(D16+$D$9)*1.6738+1651.2</f>
+        <f>(D16+$D$9)*1.6738+1651.2</f>
         <v>6458.3535999999995</v>
       </c>
       <c r="F16">
@@ -4185,7 +4235,7 @@
         <v>2400</v>
       </c>
       <c r="E17">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="E16:E41" si="1">(D17+$D$9)*1.6738+1651.2</f>
         <v>6290.9735999999994</v>
       </c>
       <c r="F17">

</xml_diff>